<commit_message>
edit file import template
</commit_message>
<xml_diff>
--- a/templates/Import-template-hidemyacc.xlsx
+++ b/templates/Import-template-hidemyacc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\xlsx-populate\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beatrix\Project\Hidemyacc\hma\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B861FB18-939C-4B95-8DAA-9E71B3401CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD29FDA-3986-411C-A023-9E2B007084C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Profile name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Example. Available formats</t>
-  </si>
-  <si>
-    <t>json</t>
   </si>
   <si>
     <t>http/socks4/socks5/ssh</t>
@@ -94,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,17 +100,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -125,7 +124,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEAD1DC"/>
+        <fgColor rgb="FF01162B"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -147,22 +147,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF01162B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,71 +445,68 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="44.42578125" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="23.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.75">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="409.6">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>